<commit_message>
Reusable method created to product page
</commit_message>
<xml_diff>
--- a/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
+++ b/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="6950" activeTab="3"/>
+    <workbookView windowWidth="18530" windowHeight="6950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="userCredentials" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="checkoutInfo" sheetId="4" r:id="rId4"/>
     <sheet name="checkoutOverview" sheetId="5" r:id="rId5"/>
     <sheet name="checkoutComplete" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>Accepted usernames and Password for all users</t>
   </si>
@@ -60,6 +61,21 @@
     <t>PRODUCTS</t>
   </si>
   <si>
+    <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
     <t>Your Cart</t>
   </si>
   <si>
@@ -72,6 +88,33 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
+    <t>A red light isn't the desired state in testing but it sure helps when riding your bike at night. Water-resistant with 3 lighting modes, 1 AAA battery included.</t>
+  </si>
+  <si>
+    <t>$9.99</t>
+  </si>
+  <si>
+    <t>Get your testing superhero on with the Sauce Labs bolt T-shirt. From American Apparel, 100% ringspun combed cotton, heather gray with red bolt.</t>
+  </si>
+  <si>
+    <t>$15.99</t>
+  </si>
+  <si>
+    <t>It's not every day that you come across a midweight quarter-zip fleece jacket capable of handling everything from a relaxing day outdoors to a busy day at the office.</t>
+  </si>
+  <si>
+    <t>$49.99</t>
+  </si>
+  <si>
+    <t>Rib snap infant onesie for the junior automation engineer in development. Reinforced 3-snap bottom closure, two-needle hemmed sleeved and bottom won't unravel.</t>
+  </si>
+  <si>
+    <t>$7.99</t>
+  </si>
+  <si>
+    <t>This classic Sauce Labs t-shirt is perfect to wear when cozying up to your keyboard to automate a few tests. Super-soft and comfy ringspun combed cotton.</t>
+  </si>
+  <si>
     <t>Checkout: Your Information</t>
   </si>
   <si>
@@ -130,17 +173,27 @@
   </si>
   <si>
     <t>Back Home</t>
+  </si>
+  <si>
+    <t>Product Title</t>
+  </si>
+  <si>
+    <t>Product Discription</t>
+  </si>
+  <si>
+    <t>Product Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -165,69 +218,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,7 +235,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,6 +293,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -271,8 +323,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,36 +341,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,187 +371,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,7 +575,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,30 +619,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -571,6 +630,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,170 +668,167 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1103,7 +1168,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1151,19 +1216,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="126.363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1185,6 +1250,36 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1196,35 +1291,35 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="126.363636363636" customWidth="1"/>
+    <col min="1" max="1" width="155.909090909091" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
+      <c r="A1" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1240,6 +1335,81 @@
     <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1423,7 @@
   <sheetPr/>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1264,38 +1434,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
+      <c r="A1" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>632510</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1320,53 +1490,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
+      <c r="A1" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="15.5" spans="1:1">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
+      <c r="A3" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1390,28 +1560,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
+      <c r="A1" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="30.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="155.909090909091" customWidth="1"/>
+    <col min="3" max="3" width="12.8181818181818" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created a meathod to add One product added without parameter
</commit_message>
<xml_diff>
--- a/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
+++ b/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Accepted usernames and Password for all users</t>
   </si>
@@ -52,40 +52,37 @@
     <t>Sauce Labs Backpack</t>
   </si>
   <si>
+    <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>Sauce Labs Bolt T-Shirt</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>Your Cart</t>
+  </si>
+  <si>
+    <t>YOUR CART</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
     <t>carry.allTheThings() with the sleek, streamlined Sly Pack that melds uncompromising style with unequaled laptop and tablet protection.</t>
   </si>
   <si>
     <t>$29.99</t>
-  </si>
-  <si>
-    <t>PRODUCTS</t>
-  </si>
-  <si>
-    <t>Sauce Labs Bike Light</t>
-  </si>
-  <si>
-    <t>Sauce Labs Bolt T-Shirt</t>
-  </si>
-  <si>
-    <t>Sauce Labs Fleece Jacket</t>
-  </si>
-  <si>
-    <t>Sauce Labs Onesie</t>
-  </si>
-  <si>
-    <t>Test.allTheThings() T-Shirt (Red)</t>
-  </si>
-  <si>
-    <t>Your Cart</t>
-  </si>
-  <si>
-    <t>YOUR CART</t>
-  </si>
-  <si>
-    <t>QTY</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
   </si>
   <si>
     <t>A red light isn't the desired state in testing but it sure helps when riding your bike at night. Water-resistant with 3 lighting modes, 1 AAA battery included.</t>
@@ -189,10 +186,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="22">
@@ -218,9 +215,61 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,50 +284,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -293,23 +298,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,32 +337,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,181 +380,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,6 +565,47 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -589,32 +627,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,47 +665,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -682,139 +685,133 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1216,13 +1213,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="2" width="126.363636363636" customWidth="1"/>
   </cols>
@@ -1254,32 +1251,12 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1293,8 +1270,8 @@
   <sheetPr/>
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1304,22 +1281,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1329,87 +1306,87 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1435,22 +1412,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1460,12 +1437,12 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1491,52 +1468,52 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" ht="15.5" spans="1:1">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1561,27 +1538,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1608,13 +1585,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1622,65 +1599,65 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All items verified Code
</commit_message>
<xml_diff>
--- a/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
+++ b/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="6950" activeTab="1"/>
+    <workbookView windowWidth="18530" windowHeight="6950" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="userCredentials" sheetId="1" r:id="rId1"/>
@@ -189,8 +189,8 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="179" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -216,13 +216,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -233,6 +226,45 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -244,21 +276,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,9 +286,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -290,24 +307,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,44 +358,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -380,181 +380,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,12 +568,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -594,35 +627,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,42 +665,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -691,138 +691,138 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -830,6 +830,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1215,7 +1218,7 @@
   <sheetPr/>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1268,10 +1271,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1300,92 +1303,122 @@
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>9</v>
+      <c r="A5" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>23</v>
+      <c r="A12" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>24</v>
+      <c r="A13" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>13</v>
+      <c r="A17" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>29</v>
+      <c r="A21" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel data Read Updated
</commit_message>
<xml_diff>
--- a/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
+++ b/SauceDemo/src/main/resources/moduleOneTestData/sauceDemoTestData.xlsx
@@ -187,10 +187,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -215,6 +215,87 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,10 +304,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -238,26 +328,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -269,88 +344,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -358,6 +351,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -380,55 +380,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,121 +554,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,10 +570,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -597,8 +595,49 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,47 +660,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -682,136 +682,136 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -825,7 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="3"/>

</xml_diff>